<commit_message>
update logische testgevallen voor upload, update, en dataset content
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>US</t>
   </si>
@@ -43,23 +43,13 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Kenniskluis/Datasets Tax X.ttl</t>
-  </si>
-  <si>
     <t>admin --&gt; upload --&gt; upload dataset-metadata (RDF of Turtle)</t>
   </si>
   <si>
     <t>Testbestand wordt geupload</t>
   </si>
   <si>
-    <t>- de datasets zijn zichtbaar op pagina Overzicht Datasets
-- er staat informatie over de upload op de detailpagina's met metadata van de datasets</t>
-  </si>
-  <si>
     <t>admin --&gt; upload --&gt; upload status (RDF of Turtle)</t>
-  </si>
-  <si>
-    <t>Kenniskluis/status X.ttl</t>
   </si>
   <si>
     <t>- login als admin</t>
@@ -69,44 +59,63 @@
 - login als admin</t>
   </si>
   <si>
-    <t>- er is een graph aangemaakt /container/statusupload</t>
-  </si>
-  <si>
     <t>admin --&gt; upload --&gt;  upload concepten (RDF of Turtle)</t>
-  </si>
-  <si>
-    <t>Kenniskluis/Testdata Tax X.ttl</t>
-  </si>
-  <si>
-    <t>- de concepten zijn zichtbaar op de pagina Alle Concepten
-- de concepten zijn zichtbaar op de pagina van de dataset</t>
-  </si>
-  <si>
-    <t>- regressietest 1 is uitgevoerd
-- login als admin</t>
-  </si>
-  <si>
-    <t>Kenniskluis/Testdata Tax Y.ttl</t>
-  </si>
-  <si>
-    <t>- Testdata Tax X is geupload
-- login als admin</t>
   </si>
   <si>
     <t xml:space="preserve">1. Testbestand X wordt geupload
 2. Testbestand wordt gesynct (upload --&gt; sync geuploade concepten naar dataset) </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Testbestand Y wordt geupload
-2. Testbestand wordt gesynct (upload --&gt; sync geuploade concepten naar dataset) </t>
+    <t>GCO-480</t>
   </si>
   <si>
-    <t>- de concepten uit testbestand X zijn afgesloten en niet meer zichtbaar in de kenniskluis
-- de concepten uit testbestand Y zijn zichtbaar op Alle Concepten
-- de concepten uit testbestand Y zijn zichtbaar op de dataset-pagina</t>
+    <t>Kenniskluis/Datasets Tax X.ttl
+Kenniskluis/Testdata Tax X.ttl</t>
   </si>
   <si>
-    <t>GCO-480</t>
+    <t>- datasets Tax is geupload (upload --&gt; upload dataset-metadata)
+- login als admin</t>
+  </si>
+  <si>
+    <t>admin --&gt; update --&gt;  upload concepten (RDF of Turtle)</t>
+  </si>
+  <si>
+    <t>- upload successful</t>
+  </si>
+  <si>
+    <t>Kenniskluis/status.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Datasets Tax T.ttl
+Kenniskluis/Testdata Tax T.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Datasets Tax.ttl</t>
+  </si>
+  <si>
+    <t>admin --&gt; overzicht datasets</t>
+  </si>
+  <si>
+    <t>- testbestand is geupload (upload --&gt; upload dataset-metadata)
+- login als admin</t>
+  </si>
+  <si>
+    <t>Als ik op de pagina kijk</t>
+  </si>
+  <si>
+    <t>dan moet ik een overzicht zien van alle datasets met een korte uitleg</t>
+  </si>
+  <si>
+    <t>Als ik op de volgende links klik:
+- Begrippen BAG
+- Begrippen BRK
+- Begrippen intern BRK (niet-juridisch)
+- Begrippen BRK intern (juridisch)
+- Begrippen BRT
+- Begrippen Tax</t>
+  </si>
+  <si>
+    <t>dan moet ik bij elke pagina de metadata van de desbetreffende dataset zien. Ook moet een tabel worden getoond met vorige versies.</t>
   </si>
 </sst>
 </file>
@@ -645,7 +654,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,27 +702,27 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" ht="72.599999999999994" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" s="21" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -722,88 +731,112 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" s="16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="16" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="B8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="16">

</xml_diff>

<commit_message>
logische testen, en aanpassing indeling testdata
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>US</t>
   </si>
@@ -55,10 +55,6 @@
     <t>- login als admin</t>
   </si>
   <si>
-    <t>- Er zijn geen concepten aanwezig bij start test 
-- login als admin</t>
-  </si>
-  <si>
     <t>admin --&gt; upload --&gt;  upload concepten (RDF of Turtle)</t>
   </si>
   <si>
@@ -77,19 +73,6 @@
   </si>
   <si>
     <t>- upload successful</t>
-  </si>
-  <si>
-    <t>Kenniskluis/Datasets Tax T.ttl</t>
-  </si>
-  <si>
-    <t>Kenniskluis/status.ttl</t>
-  </si>
-  <si>
-    <t>Kenniskluis/Datasets Tax T.ttl
-Kenniskluis/Testdata Tax T.ttl</t>
-  </si>
-  <si>
-    <t>Kenniskluis/Datasets Tax.ttl</t>
   </si>
   <si>
     <t>admin --&gt; overzicht datasets</t>
@@ -123,13 +106,37 @@
     <t>dan moet ik naar de welkomstboodschap in de hoofdpagina geleid worden</t>
   </si>
   <si>
-    <t>dan moet ik naar de detailpagina van de desbetreffende dataset worden geleid</t>
-  </si>
-  <si>
     <t>admin --&gt; overzicht datasets --&gt; begrippen BAG</t>
   </si>
   <si>
     <t>dan moet ik de metadata zien betreffende het conceptscheme van BAG, inclusief een tabel met andere versies</t>
+  </si>
+  <si>
+    <t>- login als admin
+- testdata X is geupload</t>
+  </si>
+  <si>
+    <t>- Er zijn geen concepten aanwezig 
+- login als admin</t>
+  </si>
+  <si>
+    <t>dan moet ik naar de detailpagina van de desbetreffende dataset worden geleid (check header)</t>
+  </si>
+  <si>
+    <t>GCO-323</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/Datasets Tax.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/status.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/Datasets Tax.ttl
+Kenniskluis/Regressietest/Testdata Tax T.ttl</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -290,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -357,6 +364,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +675,10 @@
   <dimension ref="A1:G405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,7 +686,7 @@
     <col min="1" max="1" width="9.109375" style="20"/>
     <col min="2" max="2" width="15.33203125" style="18" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" style="21" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" style="22" customWidth="1"/>
     <col min="6" max="7" width="35.6640625" style="20" customWidth="1"/>
     <col min="8" max="16384" width="9.109375" style="18"/>
@@ -716,48 +726,50 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -765,22 +777,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -788,119 +800,118 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>23</v>
+      <c r="B8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="B9" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11">

</xml_diff>

<commit_message>
logische testgevallen + testdata rapportages
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="202">
   <si>
     <t>US</t>
   </si>
@@ -115,11 +115,6 @@
   </si>
   <si>
     <t>DetailLink</t>
-  </si>
-  <si>
-    <t>Op de pagina is een tabel te zien metde volgende rijen (dataset | uitleg):
-Begrippen BAG | Deze dataset bevat de begrippen van de BAG.
-Begrippen TAX | Deze dataset bevat de begrippen van de TAX.</t>
   </si>
   <si>
     <t>DetailHerhaaldeUpload</t>
@@ -239,16 +234,6 @@
 vos | Ter validatie</t>
   </si>
   <si>
-    <t>Op de pagina is een tabel te zien met 6 rijen
-(Concept | Status):
-walvis | Afgekeurd
-giraffe | Gevalideerd
-hond | Geverifieerd
-kop | Niet beoordeeld
-vos | Ter afkeuring
-beer | Ter validatie</t>
-  </si>
-  <si>
     <t>Op de pagina is een tabel te zien met 2 rijen 
 (Subject | Relatie | Object):
 hond | gerelateerd aan | walvis
@@ -261,9 +246,6 @@
 hond | gerelateerd aan | walvis</t>
   </si>
   <si>
-    <t>Op de pagina is een tabel te zien met 13 rijen, zie expected results MissingLinksRapportage</t>
-  </si>
-  <si>
     <t>Expected results</t>
   </si>
   <si>
@@ -436,9 +418,6 @@
     <t>pagina /query/whereused?term= wordt bekeken</t>
   </si>
   <si>
-    <t>Op de pagina is een tabel te zijn met 13 rijen, zie expected results WhereUsedRapportage</t>
-  </si>
-  <si>
     <t>concept</t>
   </si>
   <si>
@@ -489,10 +468,250 @@
   <si>
     <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
 2. Kenniskluis/Regressietest/WhereUsedRapportage.ttl
-3. Kenniskluis/Regressietest/WhereUsedRapportage.ttl</t>
-  </si>
-  <si>
-    <t>Op de pagina is een tabel te zijn met 11 rijen, zie expected results WhereUsedRapportageHerhaaldeUpload</t>
+3. Kenniskluis/Regressietest/WhereUsedRapportageHerhaaldeUpload.ttl</t>
+  </si>
+  <si>
+    <t>- testbestanden 1 en 2 zijn geupload
+- rapportage is gesorteerd op kolom 'referentie'</t>
+  </si>
+  <si>
+    <t>- Testbestand 3. wordt geupload
+- rapportage wordt gesorteerd op kolom 'referentie'</t>
+  </si>
+  <si>
+    <t>beesten</t>
+  </si>
+  <si>
+    <t>Lid van</t>
+  </si>
+  <si>
+    <t>NietGevalideerdeLinks</t>
+  </si>
+  <si>
+    <t>/query/nietgevalideerdelinks</t>
+  </si>
+  <si>
+    <t>RapportageAfgekeurd</t>
+  </si>
+  <si>
+    <t>/id/collectie/beesten</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageAfgekeurd.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>RapportageGevalideerd</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageGevalideerd.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>pagina /query/nietgevalideerdelinks wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is een lege tabel te zien met headers:
+(Type | Status Frame | Foutieve Frame | Referentie | Niet-gevalideerde Referentie | FR_status)</t>
+  </si>
+  <si>
+    <t>RapportageGeverifieerd</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageGeverifieerd.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>RapportageTerAfkeuring</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageTerAfkeuring.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>RapportageTerValidatie</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageTerValidatie.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>RapportageNietBeoordeeld</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageNietBeoordeeld.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl</t>
+  </si>
+  <si>
+    <t>testbestand 2 uploaden</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results MissingLinksRapportage</t>
+  </si>
+  <si>
+    <t>OverzichtUpdate</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/DatasetsDetail.ttl</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
+Begrippen TAX | Deze dataset bevat de begrippen van de TAX.</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
+Begrippen BAG | Deze dataset bevat de begrippen van de BAG.
+Begrippen TAX | Deze dataset bevat de begrippen van de TAX.</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 6 rijen
+(Concept | Status):
+hond | Afgekeurd
+giraffe | Gevalideerd
+walvis | Geverifieerd
+kop | Niet beoordeeld
+vos | Ter afkeuring
+beer | Ter validatie</t>
+  </si>
+  <si>
+    <t>niet-gevalideerde referentie</t>
+  </si>
+  <si>
+    <t>FR_status</t>
+  </si>
+  <si>
+    <t>Ter afkeuring</t>
+  </si>
+  <si>
+    <t>RapportageUpdate</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageUpdateStart.ttl
+3. Kenniskluis/Regressietest/UploadStatus.ttl
+4. Kenniskluis/Regressietest/NietGevalideerdeLinksRapportageUpdate.ttl</t>
+  </si>
+  <si>
+    <t>- testbestanden 1 t/m3 zijn geupload</t>
+  </si>
+  <si>
+    <t>- testbestand 4. wordt geupload
+- pagina /query/nietgevalideerdelinks wordt bekeken
+- rapportage is gesorteerd op kolom 'referentie'</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met headers en rijen:
+(Type | Status Frame | Foutieve Frame | Referentie | Niet-gevalideerde Referentie | FR_status)
+Concept | Gevalideerd | Hond | is specialisatie van | dier | afgekeurd
+Concept | Gevalideerd | Hond | zie ook | kat | ter validatie</t>
+  </si>
+  <si>
+    <t>Looping</t>
+  </si>
+  <si>
+    <t>GCO-410</t>
+  </si>
+  <si>
+    <t>/query/loopingcontrole</t>
+  </si>
+  <si>
+    <t>pagina /query/loopingcontrole wordt bekeken</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/LoopingRapportage.ttl</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results WhereUsedRapportage</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 12 rijen, zie expected results WhereUsedRapportageHerhaaldeUpload</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results NietGevalideerdeRapportageTerAfkeuring</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results NietGevalideerdeRapportageTerAfkeuring, maar FR_status is Afgekeurd</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results NietGevalideerdeRapportageTerAfkeuring, maar FR_status is Ter validatie</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 14 rijen, zie expected results NietGevalideerdeRapportageTerAfkeuring, maar FR_status is Niet beoordeeld</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 28 rijen, zie expected results LoopingRapportage</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>- testbestanden zijn geupload
+- rapportage is gesorteerd op kolom 'link'</t>
+  </si>
+  <si>
+    <t>bestaat uit</t>
+  </si>
+  <si>
+    <t>breder dan</t>
+  </si>
+  <si>
+    <t>enger dan</t>
+  </si>
+  <si>
+    <t>heeft als actor</t>
+  </si>
+  <si>
+    <t>heeft als agent</t>
+  </si>
+  <si>
+    <t>heeft als object</t>
+  </si>
+  <si>
+    <t>heeft betrekking op</t>
+  </si>
+  <si>
+    <t>is generalisatie van</t>
+  </si>
+  <si>
+    <t>is hetzelfde als</t>
+  </si>
+  <si>
+    <t>is onderdeel van</t>
+  </si>
+  <si>
+    <t>is ongeveer hetzelfde als</t>
+  </si>
+  <si>
+    <t>is specialisatie van</t>
+  </si>
+  <si>
+    <t>lid van</t>
+  </si>
+  <si>
+    <t>zie ook</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/LoopingRapportage.ttl
+3. Kenniskluis/Regressietest/LoopingRapportageHerhaaldeUpload.ttl</t>
+  </si>
+  <si>
+    <t>- testbestanden 1 en 2 zijn geupload</t>
+  </si>
+  <si>
+    <t>- testbestand 3. wordt geupload
+- rapportage is gesorteerd op kolom 'link'</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met 16 rijen, zie expected results LoopingRapportageHerhaaldeUpload</t>
   </si>
 </sst>
 </file>
@@ -524,7 +743,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -650,38 +869,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -708,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -802,24 +995,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1130,22 +1317,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="I21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.77734375" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.88671875" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="93.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.88671875" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="119.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
@@ -1209,7 +1396,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>21</v>
@@ -1241,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>23</v>
@@ -1250,10 +1437,10 @@
         <v>22</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>10</v>
@@ -1273,7 +1460,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>21</v>
@@ -1282,48 +1469,48 @@
         <v>22</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>31</v>
+      <c r="C6" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="H6" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -1331,13 +1518,13 @@
         <v>24</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>40</v>
+      <c r="E7" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>28</v>
@@ -1346,16 +1533,16 @@
         <v>22</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -1363,92 +1550,92 @@
         <v>24</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I8" s="25" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>61</v>
+      <c r="H10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -1459,60 +1646,60 @@
         <v>25</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>10</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>54</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1520,300 +1707,480 @@
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>117</v>
+        <v>47</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>12</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>104</v>
+      <c r="H14" s="27" t="s">
+        <v>113</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>13</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="F15" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>103</v>
+      <c r="H15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>14</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>119</v>
+      <c r="H16" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>15</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>16</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>17</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>18</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>19</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>20</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>21</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
@@ -1863,6 +2230,13 @@
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
@@ -1870,13 +2244,6 @@
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -2010,12 +2377,13 @@
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -2023,13 +2391,12 @@
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="18">
@@ -7107,906 +7474,1768 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56:G56"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="32"/>
+    <col min="1" max="1" width="19.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="33">
-        <v>12</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="G2" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D3" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D4" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D15" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D16" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="42" t="s">
+      <c r="D18" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="H18" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="I18" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="42" t="s">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="E19" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E3" s="32" t="s">
+      <c r="F19" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="H20" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="H23" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D27" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D29" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D32" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="F34" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E4" s="32" t="s">
+      <c r="F37" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D40" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D41" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D42" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D43" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D44" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D45" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D48" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D49" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F49" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D50" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D51" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D52" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="F52" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D53" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D54" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D55" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D56" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D57" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D58" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D59" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G61" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="H61" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="I61" s="40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="D62" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H62" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="I62" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="D63" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G63" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H63" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="I63" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="D64" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G64" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H64" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="I64" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D65" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G65" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H65" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I65" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D66" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H66" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="I66" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D67" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G67" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H67" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="I67" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D68" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G68" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E6" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="41" t="s">
+      <c r="H68" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="I68" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D69" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E69" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G69" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H69" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I69" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D70" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G70" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E7" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="41" t="s">
+      <c r="H70" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="I70" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D71" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G71" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="H71" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="I71" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D72" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G72" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="H72" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="I72" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D73" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E73" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G73" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E8" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="41" t="s">
+      <c r="H73" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="I73" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D74" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E74" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G74" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H74" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="I74" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D75" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E75" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F75" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G75" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E9" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E10" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E11" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E12" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E13" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E14" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E15" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
-        <v>13</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E18" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E19" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I19" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E20" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E21" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E22" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E23" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E24" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I24" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E25" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E26" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E27" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="J27" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E28" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="I28" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="J28" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="18">
-        <v>14</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="31" t="s">
+      <c r="H75" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="I75" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F77" s="31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D78" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E78" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D79" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D80" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="F80" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="42" t="s">
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D81" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E81" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D82" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="E82" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D83" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E83" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D84" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E84" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="F84" s="32" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E31" s="32" t="s">
+    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D85" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D86" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E86" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F86" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E32" s="32" t="s">
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D87" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E87" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F87" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D88" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E88" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F88" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F32" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="32" t="s">
+    </row>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D89" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E89" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F89" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D90" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="32" t="s">
+      <c r="E90" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F90" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D91" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E91" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F91" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D92" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F92" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="F34" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="32" t="s">
+    </row>
+    <row r="93" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D93" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E93" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F93" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D94" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F94" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="F35" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E36" s="32" t="s">
+    </row>
+    <row r="95" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D95" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E95" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F95" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D96" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="F36" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E37" s="32" t="s">
+      <c r="E96" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F96" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D97" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E97" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F97" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D98" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E98" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F98" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="32" t="s">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D99" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E99" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F99" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D100" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E100" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="F100" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D101" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="F101" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D102" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E102" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F102" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D103" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E103" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F103" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D104" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E104" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F104" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F38" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E39" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E40" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="G41" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="G42" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E43" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="18">
-        <v>14</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E45" s="31" t="s">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D105" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F105" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D107" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F107" s="31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D108" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="F108" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E47" s="32" t="s">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D109" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="F109" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D110" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="F110" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F47" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E48" s="32" t="s">
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D111" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E111" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="F111" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D112" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F48" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="G48" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="32" t="s">
+      <c r="E112" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F112" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D113" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E113" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F113" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D114" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E114" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F114" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="F49" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="G49" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="32" t="s">
+    </row>
+    <row r="115" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D115" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F115" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D116" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E116" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F116" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="F50" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="G50" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" s="32" t="s">
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D117" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E117" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F117" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D118" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="F51" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="G51" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="32" t="s">
+      <c r="E118" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F118" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D119" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E119" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F119" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D120" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E120" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F120" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="F52" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="G52" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F53" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="G53" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="G54" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F56" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="G56" s="32" t="s">
-        <v>75</v>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D121" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F121" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D122" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F122" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D123" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E123" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F123" s="32" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A3:J15">
-    <sortCondition ref="H3:H15"/>
+    <sortCondition ref="G3:G15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update logische testgevallen + testbestanden
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="233">
   <si>
     <t>US</t>
   </si>
@@ -772,6 +772,48 @@
   </si>
   <si>
     <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX'</t>
+  </si>
+  <si>
+    <t>Upload Turtle</t>
+  </si>
+  <si>
+    <t>Validatie label</t>
+  </si>
+  <si>
+    <t>ebadmin</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder rdfs:label bevatten."</t>
+  </si>
+  <si>
+    <t>Validatie prefLabel</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
+  </si>
+  <si>
+    <t>GCO-504</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/ValidatieLabel.ttl</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/ValidatiePrefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Validatie inScheme</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/ValidatieInScheme.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten met skos:inScheme bevatten."</t>
+  </si>
+  <si>
+    <t>Testbestand 2 wordt geupload</t>
   </si>
 </sst>
 </file>
@@ -967,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1079,6 +1121,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1386,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2388,40 +2436,101 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>30</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+      <c r="B34" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="18">

</xml_diff>

<commit_message>
logische testgevallen voor homoniemen rapportage + bijbehorende testbestanden
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="242">
   <si>
     <t>US</t>
   </si>
@@ -774,9 +774,6 @@
     <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX'</t>
   </si>
   <si>
-    <t>Upload Turtle</t>
-  </si>
-  <si>
     <t>Validatie label</t>
   </si>
   <si>
@@ -814,6 +811,54 @@
   </si>
   <si>
     <t>Testbestand 2 wordt geupload</t>
+  </si>
+  <si>
+    <t>Homoniemen</t>
+  </si>
+  <si>
+    <t>GCO-409</t>
+  </si>
+  <si>
+    <t>/query/homoniemen1</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/UploadStatus.ttl
+3. Kenniskluis/Regressietest/HomoniemenRapportage1.ttl
+4. Kenniskluis/Regressietest/HomoniemenRapportage2.ttl</t>
+  </si>
+  <si>
+    <t>- testbestand 3. wordt geupload naar 'Begrippen TAX'
+- testbestand 4. wordt geupload naar 'Begrippen BAG'
+- pagina /query/homoniemen1 wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met headers en rijen:
+(Concept | prefLabel | Populatie | Met status | Komt ook voor in | Met status)
+Hond | hond | Begrippen TAX | Gevalideerd | Begrippen BAG | Geverifieerd
+Hond | hond | Begrippen BAG | Geverifieerd | Begrippen TAX | Gevalideerd</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/UploadStatus.ttl
+3. Kenniskluis/Regressietest/HomoniemenRapportage1.ttl
+4. Kenniskluis/Regressietest/HomoniemenRapportage2.ttl
+5. Kenniskluis/Regressietest/HomoniemenRapportageHerhaaldeUpload.ttl</t>
+  </si>
+  <si>
+    <t>- de testbestanden 1 en 2 zijn  geupload
+- testbestand 3. is geupload naar 'Begrippen TAX'
+- testbestand 4. is geupload naar 'Begrippen BAG'</t>
+  </si>
+  <si>
+    <t>- testbestand 5. wordt geupload naar 'Begrippen BAG'
+- pagina /query/homoniemen1 wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met headers en rijen:
+(Concept | prefLabel | Populatie | Met status | Komt ook voor in | Met status)
+Hond | hond | Begrippen TAX | Gevalideerd | Begrippen BAG | Afgekeurd
+Hond | hond | Begrippen BAG | Afgekeurd | Begrippen TAX | Gevalideerd</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1126,6 +1171,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1434,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,31 +2489,31 @@
         <v>30</v>
       </c>
       <c r="B32" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="42" t="s">
-        <v>221</v>
-      </c>
       <c r="D32" s="43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H32" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2473,31 +2521,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>220</v>
+        <v>18</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H33" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2505,10 +2553,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>220</v>
+        <v>18</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>9</v>
@@ -2517,48 +2565,84 @@
         <v>37</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H34" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <v>33</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="H35" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
         <v>34</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
+      <c r="B36" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="18">

</xml_diff>

<commit_message>
logische testgevallen synoniemen rapportage
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="248">
   <si>
     <t>US</t>
   </si>
@@ -859,6 +859,41 @@
 (Concept | prefLabel | Populatie | Met status | Komt ook voor in | Met status)
 Hond | hond | Begrippen TAX | Gevalideerd | Begrippen BAG | Afgekeurd
 Hond | hond | Begrippen BAG | Afgekeurd | Begrippen TAX | Gevalideerd</t>
+  </si>
+  <si>
+    <t>Synoniemen</t>
+  </si>
+  <si>
+    <t>/query/synoniemen</t>
+  </si>
+  <si>
+    <t>- testbestand 3. wordt geupload naar 'Begrippen TAX'
+- testbestand 4. wordt geupload naar 'Begrippen BAG'
+- pagina /query/synoniemen wordt bekeken</t>
+  </si>
+  <si>
+    <t>- testbestand 5. wordt geupload naar 'Begrippen BAG'
+- pagina /query/synoniemen wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met headers en rijen:
+(Concept | met synoniem | in dataset | met de status | komt voor als concept | met synoniem | in dataset | met de status)
+Hond | puppy | Begrippen TAX | Gevalideerd | puppy | pup | Begrippen BAG | Geverifieerd
+Hond | puppy | Begrippen TAX | Gevalideerd | Hond | (empty)  | Begrippen BAG | Geverifieerd
+Hond | (empty)  | Begrippen BAG | Geverifieerd | Hond | puppy | Begrippen TAX | Gevalideerd
+pup | (empty) | Begrippen TAX | Gevalideerd | puppy | pup | Begrippen BAG | Geverifieerd
+puppy | pup | Begrippen BAG | Geverifieerd | Hond | puppy | Begrippen TAX | Gevalideerd
+puppy | pup| Begrippen BAG | Geverifieerd | pup | (empty) | Begrippen TAX | Gevalideerd</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met headers en rijen:
+(Concept | met synoniem | in dataset | met de status | komt voor als concept | met synoniem | in dataset | met de status)
+Hond | puppy | Begrippen TAX | Gevalideerd | puppy | pup | Begrippen BAG | Geverifieerd
+Hond | puppy | Begrippen TAX | Gevalideerd | Hond | (empty)  | Begrippen BAG | Afgekeurd
+Hond | (empty)  | Begrippen BAG | Afgekeurd | Hond | puppy | Begrippen TAX | Gevalideerd
+pup | (empty) | Begrippen TAX | Gevalideerd | puppy | pup | Begrippen BAG | Geverifieerd
+puppy | pup | Begrippen BAG | Geverifieerd | Hond | puppy | Begrippen TAX | Gevalideerd
+puppy | pup| Begrippen BAG | Geverifieerd | pup | (empty) | Begrippen TAX | Gevalideerd</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="I25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2644,33 +2679,69 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="18">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="18">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
+      <c r="B38" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="18">

</xml_diff>

<commit_message>
logische testen exporteren specifiek domein (GCO-452) + bijbehorende testgevallen
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="logische testgevallen" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="281">
   <si>
     <t>US</t>
   </si>
@@ -766,14 +766,6 @@
     <t>/query/exportsubsetbegrippen</t>
   </si>
   <si>
-    <t>- testbestand 3. wordt geupload naar 'begrippen BAG'
-- testbestand 4. wordt geupload naar 'Begrippen TAX'
-- selecteer dataset 'begrippen BAG'</t>
-  </si>
-  <si>
-    <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX'</t>
-  </si>
-  <si>
     <t>Validatie label</t>
   </si>
   <si>
@@ -895,12 +887,149 @@
 puppy | pup | Begrippen BAG | Geverifieerd | Hond | puppy | Begrippen TAX | Gevalideerd
 puppy | pup| Begrippen BAG | Geverifieerd | pup | (empty) | Begrippen TAX | Gevalideerd</t>
   </si>
+  <si>
+    <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX', zie expected results ExportSpecifiekDomein</t>
+  </si>
+  <si>
+    <t>@prefix xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix skos: &lt;http://www.w3.org/2004/02/skos/core#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix ns3: &lt;http://bp4mc2.org/elmo/def/&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix ns4: &lt;http://kadaster.basisregistraties.overheid.nl/som/def#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix n1: &lt;http://localhost:8080/catalogus/tax/id/begrip/&gt;.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>n1:hond_bag rdf:type skos:Concept;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:label "hond"@nl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:comment "Dit is een uitleg voor het concept hond"^^xsd:string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ns2:broaderGeneric n1:rendier_bag;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    skos:semanticRelation n1:rendier_tax;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    skos:prefLabel "hond_tax"@nl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ns5:validatie-annotatie "20170608 dit is een validatie annotatie"^^xsd:string</t>
+  </si>
+  <si>
+    <t>n1:rendier_bag rdf:type skos:Concept;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:label "rendier"@nl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:comment "Dit is een uitleg voor het concept rendier."^^xsd:string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    skos:prefLabel "rendier_bag"@nl</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    ns4:signature "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>32 tekens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>";</t>
+    </r>
+  </si>
+  <si>
+    <t>@prefix ns4: &lt;http://bp4mc2.org/elmo/def/&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix ns2: &lt;http://purl.org/iso25964/skos-thes#&gt;.</t>
+  </si>
+  <si>
+    <t>@prefix ns5: &lt;http://kadaster.basisregistraties.overheid.nl/som/def#&gt;.</t>
+  </si>
+  <si>
+    <t>n1:poten_bag rdf:type skos:Concept;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:label "poten"@nl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    rdfs:comment "Dit is een uitleg voor het concept poten."^^xsd:string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    skos:prefLabel "poten_bag"@nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ns2:narrowerPartitive n1:poten_bag;</t>
+  </si>
+  <si>
+    <t>SpecifiekDomeinHerhaaldeUpload</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
+2. Kenniskluis/Regressietest/UploadStatus.ttl
+3. Kenniskluis/Regressietest/ExportAlleDataConcepten1.ttl
+4. Kenniskluis/Regressietest/ExportAlleDataConcepten2.ttl
+5. Kenniskluis/Regressietest/ExportAlleDataConceptenHerhaaldeUpload.ttl</t>
+  </si>
+  <si>
+    <t>- de testbestanden 1 en 2 zijn  geupload
+- testbestand 3. is geupload naar 'Begrippen BAG'
+- testbestand 4. is geupload naar 'Begrippen TAX'</t>
+  </si>
+  <si>
+    <t>- testbestand 3. wordt geupload naar 'begrippen BAG'
+- testbestand 4. wordt geupload naar 'Begrippen TAX'
+- selecteer dataset 'begrippen BAG'  (hulpmiddelen -&gt; exporteren van specifieke dataset)</t>
+  </si>
+  <si>
+    <t>- testbestand 5. wordt geupload naar 'begrippen BAG'
+- selecteer dataset 'begrippen BAG'  (hulpmiddelen -&gt; exporteren van specifieke dataset)</t>
+  </si>
+  <si>
+    <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX', zie expected results ExportSpecifiekDomeinHerhaaldeUpload</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +1041,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1089,7 +1233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1210,6 +1354,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1517,22 +1664,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="I36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.109375" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.88671875" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="126.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="119.88671875" style="25" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
@@ -2513,10 +2660,10 @@
         <v>199</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>219</v>
+        <v>278</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -2527,28 +2674,28 @@
         <v>18</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H32" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2559,28 +2706,28 @@
         <v>18</v>
       </c>
       <c r="C33" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="43" t="s">
         <v>223</v>
-      </c>
-      <c r="D33" s="43" t="s">
-        <v>225</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H33" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2591,7 +2738,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>9</v>
@@ -2600,19 +2747,19 @@
         <v>37</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H34" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2620,31 +2767,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="G35" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H35" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2652,31 +2799,31 @@
         <v>34</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G36" s="42" t="s">
-        <v>221</v>
-      </c>
-      <c r="H36" s="44" t="s">
+      <c r="J36" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -2684,31 +2831,31 @@
         <v>35</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="G37" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H37" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I37" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -2716,46 +2863,64 @@
         <v>36</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E38" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="G38" s="42" t="s">
-        <v>221</v>
-      </c>
-      <c r="H38" s="44" t="s">
-        <v>239</v>
-      </c>
-      <c r="I38" s="4" t="s">
+      <c r="J38" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
         <v>37</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
+      <c r="B39" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
@@ -7889,16 +8054,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
@@ -9131,7 +9296,7 @@
       <c r="B77" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="34" t="s">
         <v>171</v>
       </c>
       <c r="D77" s="31" t="s">
@@ -9459,7 +9624,7 @@
       <c r="B107" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="34" t="s">
         <v>171</v>
       </c>
       <c r="D107" s="31" t="s">
@@ -9527,7 +9692,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D113" s="39" t="s">
         <v>72</v>
       </c>
@@ -9538,7 +9703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D114" s="39" t="s">
         <v>72</v>
       </c>
@@ -9549,7 +9714,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D115" s="39" t="s">
         <v>127</v>
       </c>
@@ -9560,7 +9725,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D116" s="39" t="s">
         <v>72</v>
       </c>
@@ -9571,7 +9736,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D117" s="39" t="s">
         <v>128</v>
       </c>
@@ -9582,7 +9747,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D118" s="39" t="s">
         <v>129</v>
       </c>
@@ -9593,7 +9758,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D119" s="39" t="s">
         <v>72</v>
       </c>
@@ -9604,7 +9769,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D120" s="39" t="s">
         <v>72</v>
       </c>
@@ -9615,7 +9780,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D121" s="39" t="s">
         <v>130</v>
       </c>
@@ -9626,7 +9791,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D122" s="39" t="s">
         <v>72</v>
       </c>
@@ -9637,7 +9802,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="123" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D123" s="39" t="s">
         <v>131</v>
       </c>
@@ -9647,6 +9812,267 @@
       <c r="F123" s="32" t="s">
         <v>72</v>
       </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B125" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C125" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="D125" s="45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D126" s="45" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D127" s="45" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D128" s="45" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D129" s="45" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D130" s="45" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D131" s="45" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D133" s="45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D134" s="45" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D135" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D136" s="45" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D137" s="45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D138" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D139" s="45" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D140" s="45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D141" s="45" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D142" s="45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D143" s="45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D144" s="45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D145" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D146" s="45" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D147" s="45" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B149" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C149" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="D149" s="45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D150" s="45" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D151" s="45" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D152" s="45" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D153" s="45" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D154" s="45" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D155" s="45" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D156" s="45" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D157" s="45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D158" s="45" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D159" s="45" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D160" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D161" s="45" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D162" s="45" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D163" s="45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D164" s="45" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D165" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D166" s="45" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D167" s="45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D168" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D169" s="45" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D170" s="45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D171" s="45" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D173" s="45"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D174" s="45"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D175" s="45"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D176" s="45"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D177" s="45"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D178" s="45"/>
     </row>
   </sheetData>
   <sortState ref="A3:J15">

</xml_diff>

<commit_message>
logische testgevallen export + overzichtspagina, met bijbehorende testbestanden
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="logische testgevallen" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="289">
   <si>
     <t>US</t>
   </si>
@@ -1023,6 +1023,41 @@
   </si>
   <si>
     <t>Op de pagina is een export te zien in .ttl-format van de gevalideerde concepten en relaties geupload naar 'begrippen BAG', maar geen uit 'begrippen TAX', zie expected results ExportSpecifiekDomeinHerhaaldeUpload</t>
+  </si>
+  <si>
+    <t>/query/overzichtspagina?term=</t>
+  </si>
+  <si>
+    <t>- testbestand 1 is geupload
+- testbestand 2. is geupload naar 'Begrippen TAX'</t>
+  </si>
+  <si>
+    <t>- pagina /query/overzichtspagina?term= wordt bekeken</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/OverzichtConcepten.ttl</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met headers en rijen:
+(Concept | Uitleg)
+hond | Dit is een uitleg voor het concept hond
+kop| Dit is een uitleg voor het concept kop</t>
+  </si>
+  <si>
+    <t>1. Kenniskluis/Regressietest/DatasetsDetail.ttl
+2. Kenniskluis/Regressietest/OverzichtConcepten.ttl
+3. Kenniskluis/Regressietest/OverzichtConceptenUpdate.ttl</t>
+  </si>
+  <si>
+    <t>- testbestand 3. wordt geupload naar 'Begrippen TAX'
+- pagina /query/overzichtspagina?term= wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met headers en rijen:
+(Concept | Uitleg)
+giraffe | Dit is een uitleg voor het concept giraffe
+walvis| Dit is een uitleg voor het concept walvis</t>
   </si>
 </sst>
 </file>
@@ -1664,14 +1699,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K405"/>
   <sheetViews>
-    <sheetView topLeftCell="I36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.109375" style="24" bestFit="1" customWidth="1"/>
@@ -2922,33 +2957,65 @@
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
+      <c r="B40" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
+      <c r="B41" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
+      <c r="E41" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -8056,7 +8123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+    <sheetView topLeftCell="A144" workbookViewId="0">
       <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aanpassing niet-gevalideerde links rapportage + aanpassingen logische testgevallen
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="375">
   <si>
     <t>US</t>
   </si>
@@ -1072,45 +1072,6 @@
     <t>- in menubalk op concepten -&gt; TAX wordt geklikt</t>
   </si>
   <si>
-    <t>- link naar /query/overzichtspagina?term=
-- Op de pagina is o.a. een tabel te zien met headers en rijen:
-(Concept | Uitleg)
-hond | Dit is een uitleg voor het concept hond
-walvis| Dit is een uitleg voor het concept walvis</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=brk-begrippen
-- Op de pagina is o.a. een lege tabel te zien met headers:
-(Concept | Uitleg)</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=brk-intern-juridisch-begrippen
-- Op de pagina is o.a. een lege tabel te zien met headers:
-(Concept | Uitleg)</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=brk-intern-begrippen
-- Op de pagina is o.a. een lege tabel te zien met headers:
-(Concept | Uitleg)</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=brt-begrippen
-- Op de pagina is o.a. een lege tabel te zien met headers:
-(Concept | Uitleg)</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=bag-begrippen
-- Op de pagina is o.a. een tabel te zien met headers en rijen:
-(Concept | Uitleg)
-walvis| Dit is een uitleg voor het concept walvis</t>
-  </si>
-  <si>
-    <t>- link naar /query/overzichtspagina?term=&amp;dataset=tax-begrippen
-- Op de pagina is o.a. een tabel te zien met headers en rijen:
-(Concept | Uitleg)
-hond | Dit is een uitleg voor het concept hond</t>
-  </si>
-  <si>
     <t>Pagina wordt bekeken</t>
   </si>
   <si>
@@ -1382,11 +1343,64 @@
     <t>De pagina /query/exportsubsetbegrippen wordt weergegeven in hetzelfde scherm, met header 'Selecteer dataset'</t>
   </si>
   <si>
-    <t>- Testbestand 3. wordt geupload</t>
-  </si>
-  <si>
-    <t>- testbestanden 1 en 2 zijn geupload
+    <t>- Testbestand 3. wordt geupload
 - rapportage is gesorteerd op kolom 'link'</t>
+  </si>
+  <si>
+    <t>- Op de pagina is o.a. een lege tabel te zien met headers:
+(Concept | Uitleg)</t>
+  </si>
+  <si>
+    <t>- pagina wordt bekeken</t>
+  </si>
+  <si>
+    <t>/query/overzichtspagina?term=&amp;dataset=brk-begrippen</t>
+  </si>
+  <si>
+    <t>/query/overzichtspagina?term=&amp;dataset=brk-intern-juridisch-begrippen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /query/overzichtspagina?term=&amp;dataset=brk-intern-begrippen</t>
+  </si>
+  <si>
+    <t>/query/overzichtspagina?term=&amp;dataset=brt-begrippen</t>
+  </si>
+  <si>
+    <t>- Op de pagina is o.a. een tabel te zien met headers en rijen:
+(Concept | Uitleg)
+walvis| Dit is een uitleg voor het concept walvis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /query/overzichtspagina?term=&amp;dataset=bag-begrippen</t>
+  </si>
+  <si>
+    <t>- Op de pagina is o.a. een tabel te zien met headers en rijen:
+(Concept | Uitleg)
+hond | Dit is een uitleg voor het concept hond</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /query/overzichtspagina?term=&amp;dataset=tax-begrippen</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=brk-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term= wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=brk-intern-juridisch-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=brk-intern-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=brt-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=bag-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>De pagina /query/overzichtspagina?term=&amp;dataset=tax-begrippen wordt weergegeven in hetzelfde scherm</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +1605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1727,6 +1741,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2035,10 +2052,10 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2064,7 @@
     <col min="2" max="2" width="24.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.21875" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.88671875" style="30" bestFit="1" customWidth="1"/>
@@ -2605,10 +2622,10 @@
         <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>365</v>
+        <v>197</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>174</v>
@@ -2902,7 +2919,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="49">
         <v>26</v>
       </c>
@@ -3030,7 +3047,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>30</v>
       </c>
@@ -3250,19 +3267,19 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
         <v>37</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="45" t="s">
-        <v>277</v>
+        <v>360</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>278</v>
@@ -3274,10 +3291,10 @@
         <v>224</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>279</v>
+        <v>359</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>293</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3285,14 +3302,14 @@
         <v>38</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="45" t="s">
-        <v>277</v>
+        <v>361</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>278</v>
@@ -3304,10 +3321,10 @@
         <v>224</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>287</v>
+        <v>359</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>294</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3315,14 +3332,14 @@
         <v>39</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="45" t="s">
-        <v>277</v>
+        <v>362</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>278</v>
@@ -3334,10 +3351,10 @@
         <v>224</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>288</v>
+        <v>359</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>295</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3345,14 +3362,14 @@
         <v>40</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="45" t="s">
-        <v>277</v>
+        <v>363</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>278</v>
@@ -3364,10 +3381,10 @@
         <v>224</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>289</v>
+        <v>359</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>296</v>
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3375,14 +3392,14 @@
         <v>41</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="45" t="s">
-        <v>277</v>
+        <v>365</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>278</v>
@@ -3394,10 +3411,10 @@
         <v>224</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>290</v>
+        <v>359</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>297</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3405,14 +3422,14 @@
         <v>42</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>276</v>
+        <v>20</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="45" t="s">
-        <v>277</v>
+        <v>367</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>278</v>
@@ -3424,249 +3441,249 @@
         <v>224</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>291</v>
+        <v>359</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
         <v>43</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="45" t="s">
-        <v>277</v>
+      <c r="B45" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>296</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G45" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="G45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
         <v>44</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G46" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>305</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C46" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="E46" s="47" t="s">
-        <v>303</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="43" t="s">
-        <v>311</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
         <v>45</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="43" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+      <c r="J47" s="46" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
         <v>46</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="47" t="s">
+        <v>307</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="G48" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="43" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
         <v>47</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="47" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G49" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="43" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="J49" s="46" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
         <v>48</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="47" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G50" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="43" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
         <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="G51" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="43" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="J51" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="J51" s="18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="C52" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F52" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="J52" s="18" t="s">
         <v>322</v>
-      </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="47" t="s">
-        <v>303</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G52" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="43" t="s">
-        <v>311</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="J52" s="18" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3674,14 +3691,14 @@
         <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>13</v>
@@ -3693,25 +3710,25 @@
         <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="18">
         <v>52</v>
       </c>
       <c r="B54" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>324</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>330</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>13</v>
@@ -3723,10 +3740,10 @@
         <v>13</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3734,14 +3751,14 @@
         <v>53</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>13</v>
@@ -3753,10 +3770,10 @@
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3764,14 +3781,14 @@
         <v>54</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>13</v>
@@ -3783,25 +3800,25 @@
         <v>13</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="J56" s="18" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="18">
         <v>55</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>13</v>
@@ -3813,10 +3830,10 @@
         <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
+      </c>
+      <c r="J57" s="18" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3824,14 +3841,14 @@
         <v>56</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>334</v>
+        <v>25</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>13</v>
@@ -3843,10 +3860,10 @@
         <v>13</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3854,14 +3871,14 @@
         <v>57</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>13</v>
@@ -3873,10 +3890,10 @@
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3884,14 +3901,14 @@
         <v>58</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>13</v>
@@ -3903,10 +3920,10 @@
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="J60" s="18" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3914,14 +3931,14 @@
         <v>59</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>13</v>
@@ -3933,10 +3950,10 @@
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3944,14 +3961,14 @@
         <v>60</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>13</v>
@@ -3963,10 +3980,10 @@
         <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3974,14 +3991,14 @@
         <v>61</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>227</v>
+        <v>136</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>13</v>
@@ -3993,10 +4010,10 @@
         <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4004,14 +4021,14 @@
         <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>13</v>
@@ -4023,10 +4040,10 @@
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J64" s="18" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4034,14 +4051,14 @@
         <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>13</v>
@@ -4053,10 +4070,10 @@
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4064,14 +4081,14 @@
         <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>108</v>
+        <v>328</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="21" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>13</v>
@@ -4083,125 +4100,220 @@
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="18">
         <v>65</v>
       </c>
-      <c r="B67" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="21" t="s">
-        <v>325</v>
+      <c r="B67" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E67" s="47" t="s">
+        <v>277</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G67" s="19" t="s">
-        <v>206</v>
+      <c r="G67" s="50" t="s">
+        <v>13</v>
       </c>
       <c r="H67" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="J67" s="18" t="s">
-        <v>363</v>
+      <c r="I67" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="18">
         <v>66</v>
       </c>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
+      <c r="B68" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>281</v>
+      </c>
       <c r="D68" s="20"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E68" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F68" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="18">
         <v>67</v>
       </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
+      <c r="B69" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>283</v>
+      </c>
       <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E69" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F69" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="18">
         <v>68</v>
       </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
+      <c r="B70" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>282</v>
+      </c>
       <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
+      <c r="E70" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F70" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="18">
         <v>69</v>
       </c>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
+      <c r="B71" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>284</v>
+      </c>
       <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
+      <c r="E71" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F71" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="18">
         <v>70</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
+      <c r="B72" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>285</v>
+      </c>
       <c r="D72" s="20"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
+      <c r="E72" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F72" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="18">
         <v>71</v>
       </c>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
+      <c r="B73" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>286</v>
+      </c>
       <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
+      <c r="E73" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F73" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="18">
@@ -8861,7 +8973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
where used rapportage aangepast
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -2052,10 +2052,10 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
bug fixes rapportages + aanpassing logische testgevallen upload datasets
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -552,10 +552,6 @@
   <si>
     <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
 2. Kenniskluis/Regressietest/DatasetsDetail.ttl</t>
-  </si>
-  <si>
-    <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
-Begrippen TAX | Deze dataset bevat de begrippen van de TAX.</t>
   </si>
   <si>
     <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
@@ -1401,6 +1397,11 @@
   </si>
   <si>
     <t>De pagina /query/overzichtspagina?term=&amp;dataset=tax-begrippen wordt weergegeven in hetzelfde scherm</t>
+  </si>
+  <si>
+    <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
+Begrippen BAG | Deze dataset bevat de begrippen van de BAG.
+Begrippen TAX | Deze dataset bevat alle begrippen van de TAX.</t>
   </si>
 </sst>
 </file>
@@ -2052,10 +2053,10 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2212,10 +2213,10 @@
         <v>11</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>153</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>157</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2436,7 +2437,7 @@
         <v>52</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2590,13 +2591,13 @@
         <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>116</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2622,13 +2623,13 @@
         <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2660,7 +2661,7 @@
         <v>143</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2756,7 +2757,7 @@
         <v>143</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2788,7 +2789,7 @@
         <v>143</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2820,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -2831,7 +2832,7 @@
         <v>136</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>13</v>
@@ -2840,19 +2841,19 @@
         <v>137</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="J25" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2860,31 +2861,31 @@
         <v>24</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>170</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G26" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2892,31 +2893,31 @@
         <v>25</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>170</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H27" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="18" t="s">
         <v>198</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -2924,31 +2925,31 @@
         <v>26</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="E28" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="F28" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="G28" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2959,28 +2960,28 @@
         <v>18</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H29" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2991,28 +2992,28 @@
         <v>18</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H30" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3023,7 +3024,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>9</v>
@@ -3032,19 +3033,19 @@
         <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3052,31 +3053,31 @@
         <v>30</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="F32" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="G32" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H32" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3084,31 +3085,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D33" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>219</v>
-      </c>
       <c r="F33" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="G33" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="H33" s="43" t="s">
+      <c r="I33" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3116,31 +3117,31 @@
         <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H34" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3148,31 +3149,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="H35" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="G35" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="H35" s="43" t="s">
-        <v>224</v>
-      </c>
       <c r="I35" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3180,31 +3181,31 @@
         <v>34</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="E36" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I36" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3219,22 +3220,22 @@
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="J37" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3249,22 +3250,22 @@
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3275,26 +3276,26 @@
         <v>20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="45" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3305,26 +3306,26 @@
         <v>20</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G40" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3335,26 +3336,26 @@
         <v>20</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="45" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G41" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3365,26 +3366,26 @@
         <v>20</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="45" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G42" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3395,26 +3396,26 @@
         <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="45" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G43" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3425,26 +3426,26 @@
         <v>20</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="45" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="144" x14ac:dyDescent="0.3">
@@ -3452,28 +3453,28 @@
         <v>43</v>
       </c>
       <c r="B45" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="E45" s="47" t="s">
         <v>295</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="F45" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
@@ -3481,29 +3482,29 @@
         <v>44</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G46" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
@@ -3511,29 +3512,29 @@
         <v>45</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J47" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
@@ -3541,29 +3542,29 @@
         <v>46</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G48" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
@@ -3571,29 +3572,29 @@
         <v>47</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G49" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J49" s="46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -3601,29 +3602,29 @@
         <v>48</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G50" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3631,29 +3632,29 @@
         <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G51" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3661,29 +3662,29 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H52" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3691,29 +3692,29 @@
         <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H53" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="J53" s="18" t="s">
         <v>329</v>
-      </c>
-      <c r="J53" s="18" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3721,29 +3722,29 @@
         <v>52</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H54" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I54" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="J54" s="18" t="s">
         <v>331</v>
-      </c>
-      <c r="J54" s="18" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3751,29 +3752,29 @@
         <v>53</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H55" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J55" s="18" t="s">
         <v>333</v>
-      </c>
-      <c r="J55" s="18" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3781,29 +3782,29 @@
         <v>54</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H56" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3811,29 +3812,29 @@
         <v>55</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H57" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3841,29 +3842,29 @@
         <v>56</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H58" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I58" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J58" s="18" t="s">
         <v>339</v>
-      </c>
-      <c r="J58" s="18" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3871,29 +3872,29 @@
         <v>57</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C59" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H59" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3901,29 +3902,29 @@
         <v>58</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H60" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J60" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3931,29 +3932,29 @@
         <v>59</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H61" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3961,29 +3962,29 @@
         <v>60</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H62" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3991,29 +3992,29 @@
         <v>61</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C63" s="19" t="s">
         <v>136</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H63" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4021,29 +4022,29 @@
         <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H64" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J64" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4051,29 +4052,29 @@
         <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C65" s="19" t="s">
         <v>108</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H65" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4081,29 +4082,29 @@
         <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H66" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4111,13 +4112,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="E67" s="47" t="s">
         <v>276</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E67" s="47" t="s">
-        <v>277</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>13</v>
@@ -4129,10 +4130,10 @@
         <v>13</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -4140,14 +4141,14 @@
         <v>66</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>13</v>
@@ -4159,10 +4160,10 @@
         <v>13</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4170,14 +4171,14 @@
         <v>67</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>13</v>
@@ -4189,10 +4190,10 @@
         <v>13</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4200,14 +4201,14 @@
         <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>13</v>
@@ -4219,10 +4220,10 @@
         <v>13</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -4230,14 +4231,14 @@
         <v>69</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D71" s="20"/>
       <c r="E71" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>13</v>
@@ -4249,10 +4250,10 @@
         <v>13</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -4260,14 +4261,14 @@
         <v>70</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>13</v>
@@ -4279,10 +4280,10 @@
         <v>13</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -4290,14 +4291,14 @@
         <v>71</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>13</v>
@@ -4309,10 +4310,10 @@
         <v>13</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -9914,10 +9915,10 @@
         <v>67</v>
       </c>
       <c r="H61" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="I61" s="40" t="s">
         <v>160</v>
-      </c>
-      <c r="I61" s="40" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -9939,7 +9940,7 @@
         <v>120</v>
       </c>
       <c r="I62" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -9961,7 +9962,7 @@
         <v>121</v>
       </c>
       <c r="I63" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -9983,7 +9984,7 @@
         <v>122</v>
       </c>
       <c r="I64" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -10003,7 +10004,7 @@
         <v>123</v>
       </c>
       <c r="I65" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -10023,7 +10024,7 @@
         <v>124</v>
       </c>
       <c r="I66" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -10043,7 +10044,7 @@
         <v>125</v>
       </c>
       <c r="I67" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -10063,7 +10064,7 @@
         <v>126</v>
       </c>
       <c r="I68" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -10083,7 +10084,7 @@
         <v>127</v>
       </c>
       <c r="I69" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -10103,7 +10104,7 @@
         <v>128</v>
       </c>
       <c r="I70" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -10123,7 +10124,7 @@
         <v>129</v>
       </c>
       <c r="I71" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -10143,7 +10144,7 @@
         <v>130</v>
       </c>
       <c r="I72" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -10163,7 +10164,7 @@
         <v>132</v>
       </c>
       <c r="I73" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -10183,7 +10184,7 @@
         <v>134</v>
       </c>
       <c r="I74" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -10203,18 +10204,18 @@
         <v>131</v>
       </c>
       <c r="I75" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D77" s="31" t="s">
         <v>119</v>
@@ -10223,7 +10224,7 @@
         <v>118</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -10231,7 +10232,7 @@
         <v>72</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F78" s="32" t="s">
         <v>120</v>
@@ -10242,7 +10243,7 @@
         <v>120</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F79" s="32" t="s">
         <v>72</v>
@@ -10253,7 +10254,7 @@
         <v>72</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F80" s="32" t="s">
         <v>121</v>
@@ -10264,7 +10265,7 @@
         <v>121</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F81" s="32" t="s">
         <v>72</v>
@@ -10275,7 +10276,7 @@
         <v>122</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F82" s="32" t="s">
         <v>72</v>
@@ -10286,7 +10287,7 @@
         <v>72</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F83" s="32" t="s">
         <v>122</v>
@@ -10297,7 +10298,7 @@
         <v>72</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F84" s="32" t="s">
         <v>123</v>
@@ -10308,7 +10309,7 @@
         <v>123</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F85" s="32" t="s">
         <v>72</v>
@@ -10319,7 +10320,7 @@
         <v>72</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F86" s="32" t="s">
         <v>124</v>
@@ -10330,7 +10331,7 @@
         <v>124</v>
       </c>
       <c r="E87" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F87" s="32" t="s">
         <v>72</v>
@@ -10341,7 +10342,7 @@
         <v>72</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F88" s="32" t="s">
         <v>125</v>
@@ -10352,7 +10353,7 @@
         <v>125</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F89" s="32" t="s">
         <v>72</v>
@@ -10363,7 +10364,7 @@
         <v>126</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F90" s="32" t="s">
         <v>72</v>
@@ -10374,7 +10375,7 @@
         <v>72</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F91" s="32" t="s">
         <v>126</v>
@@ -10385,7 +10386,7 @@
         <v>72</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F92" s="32" t="s">
         <v>127</v>
@@ -10396,7 +10397,7 @@
         <v>127</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F93" s="32" t="s">
         <v>72</v>
@@ -10407,7 +10408,7 @@
         <v>72</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F94" s="32" t="s">
         <v>128</v>
@@ -10418,7 +10419,7 @@
         <v>128</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F95" s="32" t="s">
         <v>72</v>
@@ -10429,7 +10430,7 @@
         <v>129</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F96" s="32" t="s">
         <v>72</v>
@@ -10440,7 +10441,7 @@
         <v>72</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F97" s="32" t="s">
         <v>129</v>
@@ -10451,7 +10452,7 @@
         <v>72</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F98" s="32" t="s">
         <v>130</v>
@@ -10462,7 +10463,7 @@
         <v>130</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F99" s="32" t="s">
         <v>72</v>
@@ -10473,7 +10474,7 @@
         <v>132</v>
       </c>
       <c r="E100" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F100" s="32" t="s">
         <v>72</v>
@@ -10484,7 +10485,7 @@
         <v>72</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F101" s="32" t="s">
         <v>132</v>
@@ -10495,7 +10496,7 @@
         <v>134</v>
       </c>
       <c r="E102" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F102" s="32" t="s">
         <v>72</v>
@@ -10506,7 +10507,7 @@
         <v>72</v>
       </c>
       <c r="E103" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F103" s="32" t="s">
         <v>134</v>
@@ -10517,7 +10518,7 @@
         <v>72</v>
       </c>
       <c r="E104" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F104" s="32" t="s">
         <v>131</v>
@@ -10528,7 +10529,7 @@
         <v>131</v>
       </c>
       <c r="E105" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F105" s="32" t="s">
         <v>72</v>
@@ -10536,13 +10537,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B107" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>119</v>
@@ -10551,7 +10552,7 @@
         <v>118</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -10559,7 +10560,7 @@
         <v>72</v>
       </c>
       <c r="E108" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F108" s="32" t="s">
         <v>121</v>
@@ -10570,7 +10571,7 @@
         <v>121</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F109" s="32" t="s">
         <v>72</v>
@@ -10581,7 +10582,7 @@
         <v>72</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F110" s="32" t="s">
         <v>125</v>
@@ -10592,7 +10593,7 @@
         <v>125</v>
       </c>
       <c r="E111" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F111" s="32" t="s">
         <v>72</v>
@@ -10603,7 +10604,7 @@
         <v>126</v>
       </c>
       <c r="E112" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F112" s="32" t="s">
         <v>72</v>
@@ -10614,7 +10615,7 @@
         <v>72</v>
       </c>
       <c r="E113" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F113" s="32" t="s">
         <v>126</v>
@@ -10625,7 +10626,7 @@
         <v>72</v>
       </c>
       <c r="E114" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F114" s="32" t="s">
         <v>127</v>
@@ -10636,7 +10637,7 @@
         <v>127</v>
       </c>
       <c r="E115" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F115" s="32" t="s">
         <v>72</v>
@@ -10647,7 +10648,7 @@
         <v>72</v>
       </c>
       <c r="E116" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F116" s="32" t="s">
         <v>128</v>
@@ -10658,7 +10659,7 @@
         <v>128</v>
       </c>
       <c r="E117" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F117" s="32" t="s">
         <v>72</v>
@@ -10669,7 +10670,7 @@
         <v>129</v>
       </c>
       <c r="E118" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F118" s="32" t="s">
         <v>72</v>
@@ -10680,7 +10681,7 @@
         <v>72</v>
       </c>
       <c r="E119" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F119" s="32" t="s">
         <v>129</v>
@@ -10691,7 +10692,7 @@
         <v>72</v>
       </c>
       <c r="E120" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F120" s="32" t="s">
         <v>130</v>
@@ -10702,7 +10703,7 @@
         <v>130</v>
       </c>
       <c r="E121" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F121" s="32" t="s">
         <v>72</v>
@@ -10713,7 +10714,7 @@
         <v>72</v>
       </c>
       <c r="E122" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F122" s="32" t="s">
         <v>131</v>
@@ -10724,7 +10725,7 @@
         <v>131</v>
       </c>
       <c r="E123" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F123" s="32" t="s">
         <v>72</v>
@@ -10732,245 +10733,245 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B125" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C125" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="B125" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C125" s="33" t="s">
-        <v>201</v>
-      </c>
       <c r="D125" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D126" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D127" s="44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D128" s="44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="44" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="44" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D145" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D146" s="44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D147" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B149" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C149" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="B149" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="C149" s="33" t="s">
-        <v>201</v>
-      </c>
       <c r="D149" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D150" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D151" s="44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D152" s="44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D153" s="44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D154" s="44" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D155" s="44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D156" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D157" s="44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D158" s="44" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D159" s="44" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D160" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161" s="44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163" s="44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164" s="44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166" s="44" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169" s="44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="173" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update logische testgevallen voor validaties
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="386">
   <si>
     <t>US</t>
   </si>
@@ -720,16 +720,10 @@
     <t>/query/exportsubsetbegrippen</t>
   </si>
   <si>
-    <t>Validatie label</t>
-  </si>
-  <si>
     <t>ebadmin</t>
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder rdfs:label bevatten."</t>
-  </si>
-  <si>
-    <t>Validatie prefLabel</t>
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
@@ -744,9 +738,6 @@
   <si>
     <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
 2. Kenniskluis/Regressietest/ValidatiePrefLabel.ttl</t>
-  </si>
-  <si>
-    <t>Validatie inScheme</t>
   </si>
   <si>
     <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
@@ -1402,6 +1393,48 @@
     <t>Op de pagina is een tabel te zien met de volgende rijen (dataset | uitleg):
 Begrippen BAG | Deze dataset bevat de begrippen van de BAG.
 Begrippen TAX | Deze dataset bevat alle begrippen van de TAX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validatie Concepten inScheme </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validatie Concepten prefLabel </t>
+  </si>
+  <si>
+    <t>Validatie Concepten Label</t>
+  </si>
+  <si>
+    <t>Validatie Datasets Title</t>
+  </si>
+  <si>
+    <t>GCO-601</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieDatasetsTitle.ttl</t>
+  </si>
+  <si>
+    <t>het testbestand wordt geupload</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen datasets zonder dct:title bevatten."</t>
+  </si>
+  <si>
+    <t>Validatie Datasets ConceptScheme</t>
+  </si>
+  <si>
+    <t>Validatie Datasets Dataset</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieDatasetsConceptScheme.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieDatasetsDataset.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen datasets zonder skos:ConceptScheme bevatten."</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen datasets zonder dcat:Dataset bevatten."</t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2086,10 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2245,7 +2278,7 @@
         <v>153</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2626,7 +2659,7 @@
         <v>196</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>173</v>
@@ -2946,10 +2979,10 @@
         <v>196</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2960,28 +2993,28 @@
         <v>18</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>204</v>
+        <v>374</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H29" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2992,28 +3025,28 @@
         <v>18</v>
       </c>
       <c r="C30" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>207</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>209</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H30" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3024,7 +3057,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>212</v>
+        <v>372</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>9</v>
@@ -3033,19 +3066,19 @@
         <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H31" s="22" t="s">
         <v>105</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3053,31 +3086,31 @@
         <v>30</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H32" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3085,31 +3118,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="H33" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3117,31 +3150,31 @@
         <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H34" s="27" t="s">
         <v>113</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3149,31 +3182,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H35" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3184,7 +3217,7 @@
         <v>199</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>200</v>
@@ -3193,19 +3226,19 @@
         <v>203</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3220,22 +3253,22 @@
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3250,22 +3283,22 @@
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3276,26 +3309,26 @@
         <v>20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="45" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3306,26 +3339,26 @@
         <v>20</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="45" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G40" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3336,26 +3369,26 @@
         <v>20</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="45" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G41" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3366,26 +3399,26 @@
         <v>20</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="45" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G42" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3396,26 +3429,26 @@
         <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="45" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G43" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3426,26 +3459,26 @@
         <v>20</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="45" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="144" x14ac:dyDescent="0.3">
@@ -3453,28 +3486,28 @@
         <v>43</v>
       </c>
       <c r="B45" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="E45" s="47" t="s">
-        <v>295</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
@@ -3482,29 +3515,29 @@
         <v>44</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G46" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="43" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
@@ -3512,29 +3545,29 @@
         <v>45</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J47" s="46" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
@@ -3542,29 +3575,29 @@
         <v>46</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="47" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G48" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
@@ -3572,29 +3605,29 @@
         <v>47</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G49" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="43" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J49" s="46" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -3602,29 +3635,29 @@
         <v>48</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G50" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3632,29 +3665,29 @@
         <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="47" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G51" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3662,29 +3695,29 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H52" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3692,29 +3725,29 @@
         <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H53" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3722,29 +3755,29 @@
         <v>52</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H54" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3752,29 +3785,29 @@
         <v>53</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H55" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3782,29 +3815,29 @@
         <v>54</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H56" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3812,29 +3845,29 @@
         <v>55</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H57" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3842,29 +3875,29 @@
         <v>56</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H58" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3872,29 +3905,29 @@
         <v>57</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C59" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H59" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3902,29 +3935,29 @@
         <v>58</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H60" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="J60" s="18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3932,29 +3965,29 @@
         <v>59</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H61" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3962,29 +3995,29 @@
         <v>60</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H62" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3992,29 +4025,29 @@
         <v>61</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C63" s="19" t="s">
         <v>136</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H63" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4022,29 +4055,29 @@
         <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C64" s="19" t="s">
         <v>167</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H64" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J64" s="18" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4052,29 +4085,29 @@
         <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C65" s="19" t="s">
         <v>108</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H65" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4082,29 +4115,29 @@
         <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H66" s="22" t="s">
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4112,13 +4145,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E67" s="47" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>13</v>
@@ -4130,10 +4163,10 @@
         <v>13</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -4141,14 +4174,14 @@
         <v>66</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>13</v>
@@ -4160,10 +4193,10 @@
         <v>13</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4171,14 +4204,14 @@
         <v>67</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>13</v>
@@ -4190,10 +4223,10 @@
         <v>13</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4201,14 +4234,14 @@
         <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>13</v>
@@ -4220,10 +4253,10 @@
         <v>13</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -4231,14 +4264,14 @@
         <v>69</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D71" s="20"/>
       <c r="E71" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>13</v>
@@ -4250,10 +4283,10 @@
         <v>13</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -4261,14 +4294,14 @@
         <v>70</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>13</v>
@@ -4280,10 +4313,10 @@
         <v>13</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -4291,14 +4324,14 @@
         <v>71</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>13</v>
@@ -4310,53 +4343,107 @@
         <v>13</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="18">
         <v>72</v>
       </c>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
+      <c r="B74" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="G74" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H74" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>73</v>
       </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
+      <c r="B75" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H75" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="18">
         <v>74</v>
       </c>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
+      <c r="B76" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I76" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
@@ -10742,112 +10829,112 @@
         <v>200</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D126" s="44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D127" s="44" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D128" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="44" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="44" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="44" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="44" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="44" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="44" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="44" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="44" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="44" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="44" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D145" s="44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D146" s="44" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D147" s="44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -10855,123 +10942,123 @@
         <v>199</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C149" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D149" s="44" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D150" s="44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D151" s="44" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D152" s="44" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D153" s="44" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D154" s="44" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D155" s="44" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D156" s="44" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D157" s="44" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D158" s="44" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D159" s="44" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D160" s="44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161" s="44" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162" s="44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163" s="44" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164" s="44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165" s="44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166" s="44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167" s="44" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168" s="44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169" s="44" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170" s="44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" s="44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="173" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
regressietesten voor GCO-555 toegevoegd voor kenniskluis
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="390">
   <si>
     <t>US</t>
   </si>
@@ -723,31 +723,10 @@
     <t>ebadmin</t>
   </si>
   <si>
-    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder rdfs:label bevatten."</t>
-  </si>
-  <si>
-    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
-  </si>
-  <si>
     <t>GCO-504</t>
   </si>
   <si>
-    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
-2. Kenniskluis/Regressietest/ValidatieLabel.ttl</t>
-  </si>
-  <si>
-    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
-2. Kenniskluis/Regressietest/ValidatiePrefLabel.ttl</t>
-  </si>
-  <si>
-    <t>1. Kenniskluis/Regressietest/UploadDataset.ttl
-2. Kenniskluis/Regressietest/ValidatieInScheme.ttl</t>
-  </si>
-  <si>
     <t>Container geeft als foutmelding "De upload mag geen concepten met skos:inScheme bevatten."</t>
-  </si>
-  <si>
-    <t>Testbestand 2 wordt geupload</t>
   </si>
   <si>
     <t>Homoniemen</t>
@@ -1435,6 +1414,36 @@
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload mag geen datasets zonder dcat:Dataset bevatten."</t>
+  </si>
+  <si>
+    <t>Validatie Concepten Leeg label</t>
+  </si>
+  <si>
+    <t>Validatie Concepten Leeg prefLabel</t>
+  </si>
+  <si>
+    <t>GCO-555</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieLabel.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatiePrefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieInScheme.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder zonder of met leeg rdfs:label bevatten."</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder zonder of met leeg skos:prefLabel bevatten."</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieLeegLabel.ttl</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/ValidatieLeegPrefLabel.ttl</t>
   </si>
 </sst>
 </file>
@@ -2086,17 +2095,17 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="F61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomRight" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.21875" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" style="29" bestFit="1" customWidth="1"/>
@@ -2278,7 +2287,7 @@
         <v>153</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2659,7 +2668,7 @@
         <v>196</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>173</v>
@@ -2979,13 +2988,13 @@
         <v>196</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="49">
         <v>27</v>
       </c>
@@ -2993,31 +3002,31 @@
         <v>18</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>208</v>
+        <v>383</v>
       </c>
       <c r="G29" s="41" t="s">
         <v>204</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="49">
         <v>28</v>
       </c>
@@ -3025,31 +3034,31 @@
         <v>18</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>209</v>
+        <v>384</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>204</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>29</v>
       </c>
@@ -3057,7 +3066,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>9</v>
@@ -3066,19 +3075,19 @@
         <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>210</v>
+        <v>385</v>
       </c>
       <c r="G31" s="41" t="s">
         <v>204</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3086,19 +3095,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G32" s="41" t="s">
         <v>204</v>
@@ -3107,10 +3116,10 @@
         <v>113</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3118,31 +3127,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G33" s="41" t="s">
         <v>204</v>
       </c>
       <c r="H33" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3150,19 +3159,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G34" s="41" t="s">
         <v>204</v>
@@ -3171,10 +3180,10 @@
         <v>113</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -3182,31 +3191,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G35" s="41" t="s">
         <v>204</v>
       </c>
       <c r="H35" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>226</v>
-      </c>
       <c r="J35" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -3217,7 +3226,7 @@
         <v>199</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>200</v>
@@ -3226,19 +3235,19 @@
         <v>203</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="43" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3253,22 +3262,22 @@
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3283,22 +3292,22 @@
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="21" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3309,26 +3318,26 @@
         <v>20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="45" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3339,26 +3348,26 @@
         <v>20</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="45" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G40" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3369,26 +3378,26 @@
         <v>20</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="45" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G41" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3399,26 +3408,26 @@
         <v>20</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="45" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G42" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3429,26 +3438,26 @@
         <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="45" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G43" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -3459,26 +3468,26 @@
         <v>20</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="45" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G44" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="144" x14ac:dyDescent="0.3">
@@ -3486,28 +3495,28 @@
         <v>43</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E45" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
@@ -3515,29 +3524,29 @@
         <v>44</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G46" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="43" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
@@ -3545,29 +3554,29 @@
         <v>45</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G47" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J47" s="46" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
@@ -3575,29 +3584,29 @@
         <v>46</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="47" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G48" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
@@ -3605,29 +3614,29 @@
         <v>47</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G49" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="43" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J49" s="46" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -3635,29 +3644,29 @@
         <v>48</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G50" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3665,29 +3674,29 @@
         <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G51" s="48" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3695,14 +3704,14 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>13</v>
@@ -3714,10 +3723,10 @@
         <v>13</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3725,14 +3734,14 @@
         <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" s="19" t="s">
         <v>313</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>319</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>13</v>
@@ -3744,10 +3753,10 @@
         <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3755,14 +3764,14 @@
         <v>52</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>13</v>
@@ -3774,10 +3783,10 @@
         <v>13</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3785,14 +3794,14 @@
         <v>53</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>13</v>
@@ -3804,10 +3813,10 @@
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3815,14 +3824,14 @@
         <v>54</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>13</v>
@@ -3834,10 +3843,10 @@
         <v>13</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3845,14 +3854,14 @@
         <v>55</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>13</v>
@@ -3864,10 +3873,10 @@
         <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3875,14 +3884,14 @@
         <v>56</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>13</v>
@@ -3894,10 +3903,10 @@
         <v>13</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3905,14 +3914,14 @@
         <v>57</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C59" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>13</v>
@@ -3924,10 +3933,10 @@
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3935,14 +3944,14 @@
         <v>58</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>13</v>
@@ -3954,10 +3963,10 @@
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="J60" s="18" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3965,14 +3974,14 @@
         <v>59</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>13</v>
@@ -3984,10 +3993,10 @@
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3995,14 +4004,14 @@
         <v>60</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>13</v>
@@ -4014,10 +4023,10 @@
         <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4025,14 +4034,14 @@
         <v>61</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C63" s="19" t="s">
         <v>136</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>13</v>
@@ -4044,10 +4053,10 @@
         <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4055,14 +4064,14 @@
         <v>62</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C64" s="19" t="s">
         <v>167</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>13</v>
@@ -4074,10 +4083,10 @@
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="J64" s="18" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4085,14 +4094,14 @@
         <v>63</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C65" s="19" t="s">
         <v>108</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>13</v>
@@ -4104,10 +4113,10 @@
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4115,14 +4124,14 @@
         <v>64</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>13</v>
@@ -4134,10 +4143,10 @@
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4145,13 +4154,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E67" s="47" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>13</v>
@@ -4163,10 +4172,10 @@
         <v>13</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -4174,14 +4183,14 @@
         <v>66</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>13</v>
@@ -4193,10 +4202,10 @@
         <v>13</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4204,14 +4213,14 @@
         <v>67</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>13</v>
@@ -4223,10 +4232,10 @@
         <v>13</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4234,14 +4243,14 @@
         <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>272</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>278</v>
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>13</v>
@@ -4253,10 +4262,10 @@
         <v>13</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -4264,14 +4273,14 @@
         <v>69</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D71" s="20"/>
       <c r="E71" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>13</v>
@@ -4283,10 +4292,10 @@
         <v>13</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -4294,14 +4303,14 @@
         <v>70</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>13</v>
@@ -4313,10 +4322,10 @@
         <v>13</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -4324,14 +4333,14 @@
         <v>71</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="45" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>13</v>
@@ -4343,10 +4352,10 @@
         <v>13</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -4357,16 +4366,16 @@
         <v>18</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E74" s="21" t="s">
         <v>36</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G74" s="19" t="s">
         <v>204</v>
@@ -4375,10 +4384,10 @@
         <v>13</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -4389,16 +4398,16 @@
         <v>18</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E75" s="21" t="s">
         <v>36</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="G75" s="19" t="s">
         <v>204</v>
@@ -4407,10 +4416,10 @@
         <v>13</v>
       </c>
       <c r="I75" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="J75" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -4421,16 +4430,16 @@
         <v>18</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E76" s="21" t="s">
         <v>36</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G76" s="19" t="s">
         <v>204</v>
@@ -4439,39 +4448,75 @@
         <v>13</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
         <v>75</v>
       </c>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
+      <c r="B77" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="G77" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H77" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="18">
         <v>76</v>
       </c>
-      <c r="B78" s="19"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
+      <c r="B78" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="G78" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H78" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="18">
@@ -4482,10 +4527,10 @@
       <c r="D79" s="20"/>
       <c r="E79" s="21"/>
       <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="18"/>
+      <c r="G79" s="41"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="18">
@@ -10829,112 +10874,112 @@
         <v>200</v>
       </c>
       <c r="D125" s="44" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D126" s="44" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D127" s="44" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D128" s="44" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="44" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="44" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="44" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="44" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="44" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="44" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="44" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="44" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="44" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="44" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="44" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="44" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="44" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="44" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="44" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D145" s="44" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D146" s="44" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D147" s="44" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -10942,123 +10987,123 @@
         <v>199</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C149" s="33" t="s">
         <v>200</v>
       </c>
       <c r="D149" s="44" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D150" s="44" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D151" s="44" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D152" s="44" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D153" s="44" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D154" s="44" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D155" s="44" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D156" s="44" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D157" s="44" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D158" s="44" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D159" s="44" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D160" s="44" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161" s="44" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162" s="44" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163" s="44" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164" s="44" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165" s="44" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166" s="44" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167" s="44" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168" s="44" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169" s="44" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170" s="44" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171" s="44" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="173" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
upload informatiemodellen in kenniskluis
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Kenniskluis.xlsx
+++ b/catalogusdata/Logische testen Kenniskluis.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="402">
   <si>
     <t>US</t>
   </si>
@@ -1465,6 +1465,21 @@
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload bevat geen concepten."</t>
+  </si>
+  <si>
+    <t>InformatieModel</t>
+  </si>
+  <si>
+    <t>GCO-57</t>
+  </si>
+  <si>
+    <t>/container/ttlmodelupload</t>
+  </si>
+  <si>
+    <t>Kenniskluis/Regressietest/UploadInformatiemodel.ttl</t>
+  </si>
+  <si>
+    <t>Testbestand wordt geupload naar BAG</t>
   </si>
 </sst>
 </file>
@@ -2116,10 +2131,10 @@
   <dimension ref="A1:J405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4607,15 +4622,33 @@
       <c r="A81" s="18">
         <v>79</v>
       </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
+      <c r="B81" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="H81" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J81" s="23" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="18">

</xml_diff>